<commit_message>
jpch - Added most driving commands. Drivetrain subsystem to test and finish.
</commit_message>
<xml_diff>
--- a/hardwareList.xlsx
+++ b/hardwareList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="88">
   <si>
     <t>Actionneurs</t>
   </si>
@@ -279,6 +279,15 @@
   </si>
   <si>
     <t>francois</t>
+  </si>
+  <si>
+    <t>État actuel</t>
+  </si>
+  <si>
+    <t>terminé</t>
+  </si>
+  <si>
+    <t>à tester</t>
   </si>
 </sst>
 </file>
@@ -771,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -804,6 +813,9 @@
       <c r="I1" t="s">
         <v>80</v>
       </c>
+      <c r="J1" t="s">
+        <v>85</v>
+      </c>
       <c r="O1" t="s">
         <v>20</v>
       </c>
@@ -827,6 +839,9 @@
       <c r="I3" t="s">
         <v>81</v>
       </c>
+      <c r="J3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -844,6 +859,9 @@
       <c r="I4" t="s">
         <v>81</v>
       </c>
+      <c r="J4" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -861,6 +879,9 @@
       <c r="I5" t="s">
         <v>81</v>
       </c>
+      <c r="J5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -878,6 +899,9 @@
       <c r="I6" t="s">
         <v>81</v>
       </c>
+      <c r="J6" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
@@ -891,6 +915,9 @@
       </c>
       <c r="I7" t="s">
         <v>81</v>
+      </c>
+      <c r="J7" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Work on platform subsystem and commands
</commit_message>
<xml_diff>
--- a/hardwareList.xlsx
+++ b/hardwareList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="85">
   <si>
     <t>Actionneurs</t>
   </si>
@@ -279,15 +279,6 @@
   </si>
   <si>
     <t>francois</t>
-  </si>
-  <si>
-    <t>État actuel</t>
-  </si>
-  <si>
-    <t>terminé</t>
-  </si>
-  <si>
-    <t>à tester</t>
   </si>
 </sst>
 </file>
@@ -780,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -813,9 +804,6 @@
       <c r="I1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" t="s">
-        <v>85</v>
-      </c>
       <c r="O1" t="s">
         <v>20</v>
       </c>
@@ -839,9 +827,6 @@
       <c r="I3" t="s">
         <v>81</v>
       </c>
-      <c r="J3" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -859,9 +844,6 @@
       <c r="I4" t="s">
         <v>81</v>
       </c>
-      <c r="J4" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -879,9 +861,6 @@
       <c r="I5" t="s">
         <v>81</v>
       </c>
-      <c r="J5" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -899,9 +878,6 @@
       <c r="I6" t="s">
         <v>81</v>
       </c>
-      <c r="J6" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
@@ -915,9 +891,6 @@
       </c>
       <c r="I7" t="s">
         <v>81</v>
-      </c>
-      <c r="J7" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updates planning Excel sheet.
</commit_message>
<xml_diff>
--- a/hardwareList.xlsx
+++ b/hardwareList.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fenix\workspace\robot2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Git\robot2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="85">
   <si>
     <t>Actionneurs</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Solenoid</t>
   </si>
   <si>
-    <t>pivot</t>
-  </si>
-  <si>
     <t>pivotMotor</t>
   </si>
   <si>
@@ -279,12 +276,15 @@
   </si>
   <si>
     <t>francois</t>
+  </si>
+  <si>
+    <t>pivot (en cours, francois)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -294,7 +294,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -319,6 +319,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -332,11 +338,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,7 +481,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -768,24 +776,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" customWidth="1"/>
-    <col min="8" max="8" width="26.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -799,16 +807,16 @@
         <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -822,13 +830,13 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -839,13 +847,13 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -856,13 +864,13 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -873,13 +881,13 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -887,38 +895,38 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I10" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" t="s">
         <v>82</v>
       </c>
-      <c r="J10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -929,16 +937,16 @@
         <v>8</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" t="s">
         <v>16</v>
@@ -947,23 +955,23 @@
         <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="F13" s="2"/>
       <c r="L13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -974,16 +982,16 @@
         <v>8</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" t="s">
         <v>16</v>
@@ -992,96 +1000,96 @@
         <v>10</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" t="s">
         <v>51</v>
       </c>
-      <c r="G15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="F16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" t="s">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="I18" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I19" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" t="s">
-        <v>55</v>
-      </c>
-      <c r="I20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" t="s">
-        <v>56</v>
-      </c>
-      <c r="I21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F22" t="s">
-        <v>58</v>
-      </c>
-      <c r="G22" t="s">
-        <v>57</v>
-      </c>
-      <c r="I22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>28</v>
-      </c>
-      <c r="B24" t="s">
-        <v>29</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -1090,137 +1098,152 @@
         <v>12</v>
       </c>
       <c r="F24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="I25" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
         <v>31</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F26" t="s">
+        <v>61</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="I27" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I28" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="O29" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
         <v>37</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>38</v>
       </c>
-      <c r="C30" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" t="s">
-        <v>40</v>
-      </c>
-      <c r="F31" t="s">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F32" t="s">
+      <c r="G32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>66</v>
       </c>
-      <c r="G32" t="s">
+      <c r="F36" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G37" t="s">
+        <v>69</v>
+      </c>
+      <c r="I37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>71</v>
+      </c>
+      <c r="G38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>73</v>
+      </c>
+      <c r="G39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>75</v>
+      </c>
+      <c r="G40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F42" s="3" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>67</v>
-      </c>
-      <c r="F36" t="s">
-        <v>68</v>
-      </c>
-      <c r="G36" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F37" t="s">
-        <v>69</v>
-      </c>
-      <c r="G37" t="s">
-        <v>70</v>
-      </c>
-      <c r="I37" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F38" t="s">
-        <v>72</v>
-      </c>
-      <c r="G38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F39" t="s">
-        <v>74</v>
-      </c>
-      <c r="G39" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F40" t="s">
-        <v>76</v>
-      </c>
-      <c r="G40" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F42" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>